<commit_message>
reaarange the excel cell to allow better data retrieval in excel file from pandas
</commit_message>
<xml_diff>
--- a/etl_processor/data_source/food/licensed_local_food_farm.xlsx
+++ b/etl_processor/data_source/food/licensed_local_food_farm.xlsx
@@ -1,10 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10714"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6767C3CF-E69B-1C47-A8F7-C79A07A1A4C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="27060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet sheetId="1" name="M891471" state="visible" r:id="rId4"/>
+    <sheet name="M891471" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
@@ -121,21 +125,23 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="#,0.##########"/>
-    <numFmt numFmtId="165" formatCode="#,0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="#,##0.##########"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-      <sz val="11"/>
-      <name val="Calibri"/>
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -155,10 +161,18 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -175,7 +189,7 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -516,14 +530,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F35"/>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F44"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="6" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -543,258 +562,273 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F10" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+    <row r="11" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19"/>
+      <c r="C19"/>
+      <c r="D19"/>
+      <c r="E19"/>
+      <c r="F19"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23"/>
+      <c r="C23"/>
+      <c r="D23"/>
+      <c r="E23"/>
+      <c r="F23"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A38" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B38" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C38" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D38" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E38" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="F38" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="5">
+      <c r="B39" s="5">
         <v>254</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C39" s="5">
         <v>257</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D39" s="5">
         <v>260</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E39" s="5">
         <v>237</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F39" s="5">
         <v>221</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="5">
+      <c r="B40" s="5">
         <v>98</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C40" s="5">
         <v>109</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D40" s="5">
         <v>110</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E40" s="5">
         <v>109</v>
       </c>
-      <c r="F13" s="5">
+      <c r="F40" s="5">
         <v>110</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="5">
+      <c r="B41" s="5">
         <v>33</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C41" s="5">
         <v>27</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D41" s="5">
         <v>27</v>
       </c>
-      <c r="E14" s="5">
+      <c r="E41" s="5">
         <v>22</v>
       </c>
-      <c r="F14" s="5">
+      <c r="F41" s="5">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="5">
+      <c r="B42" s="5">
         <v>115</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C42" s="5">
         <v>111</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D42" s="5">
         <v>113</v>
       </c>
-      <c r="E15" s="5">
+      <c r="E42" s="5">
         <v>96</v>
       </c>
-      <c r="F15" s="5">
+      <c r="F42" s="5">
         <v>85</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="5">
+      <c r="B43" s="5">
         <v>3</v>
       </c>
-      <c r="C16" s="5">
+      <c r="C43" s="5">
         <v>3</v>
       </c>
-      <c r="D16" s="5">
+      <c r="D43" s="5">
         <v>3</v>
       </c>
-      <c r="E16" s="5">
+      <c r="E43" s="5">
         <v>3</v>
       </c>
-      <c r="F16" s="5">
+      <c r="F43" s="5">
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="5">
+      <c r="B44" s="5">
         <v>5</v>
       </c>
-      <c r="C17" s="5">
+      <c r="C44" s="5">
         <v>7</v>
       </c>
-      <c r="D17" s="5">
+      <c r="D44" s="5">
         <v>7</v>
       </c>
-      <c r="E17" s="5">
+      <c r="E44" s="5">
         <v>7</v>
       </c>
-      <c r="F17" s="5">
+      <c r="F44" s="5">
         <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
 </worksheet>
 </file>
</xml_diff>